<commit_message>
analysis_draft2017b: updating analysis to use marc_s2 simulation data
</commit_message>
<xml_diff>
--- a/analysis_draft2017b/csv/t01.xlsx
+++ b/analysis_draft2017b/csv/t01.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
   <si>
     <t>Sulfate aerosol</t>
   </si>
@@ -82,37 +82,37 @@
     <t>Lifetime, days</t>
   </si>
   <si>
-    <t>+536.21 ± 0.92</t>
+    <t>+538.70 ± 0.75</t>
   </si>
   <si>
     <t>+0.00 ± 0.00</t>
   </si>
   <si>
-    <t>+11.94 ± 0.05</t>
-  </si>
-  <si>
-    <t>+21.87 ± 0.03</t>
-  </si>
-  <si>
-    <t>+502.39 ± 0.90</t>
-  </si>
-  <si>
-    <t>-536.38 ± 0.92</t>
-  </si>
-  <si>
-    <t>-394.12 ± 0.85</t>
-  </si>
-  <si>
-    <t>-20.67 ± 0.05</t>
-  </si>
-  <si>
-    <t>-116.38 ± 0.07</t>
-  </si>
-  <si>
-    <t>-5.22 ± 0.01</t>
-  </si>
-  <si>
-    <t>+1.32 ± 0.00</t>
+    <t>+11.55 ± 0.05</t>
+  </si>
+  <si>
+    <t>+22.33 ± 0.02</t>
+  </si>
+  <si>
+    <t>+504.82 ± 0.75</t>
+  </si>
+  <si>
+    <t>-538.88 ± 0.74</t>
+  </si>
+  <si>
+    <t>-396.60 ± 0.69</t>
+  </si>
+  <si>
+    <t>-20.75 ± 0.06</t>
+  </si>
+  <si>
+    <t>-116.29 ± 0.06</t>
+  </si>
+  <si>
+    <t>-5.25 ± 0.01</t>
+  </si>
+  <si>
+    <t>+1.33 ± 0.00</t>
   </si>
   <si>
     <t>+0.90 ± 0.00</t>
@@ -127,100 +127,103 @@
     <t>-0.00 ± 0.00</t>
   </si>
   <si>
-    <t>+0.12 ± 0.00</t>
-  </si>
-  <si>
-    <t>+0.10 ± 0.00</t>
+    <t>+0.13 ± 0.00</t>
   </si>
   <si>
     <t>+0.09 ± 0.00</t>
   </si>
   <si>
-    <t>-0.10 ± 0.00</t>
-  </si>
-  <si>
-    <t>+507.11 ± 0.90</t>
-  </si>
-  <si>
-    <t>+4.61 ± 0.02</t>
-  </si>
-  <si>
-    <t>-507.19 ± 0.90</t>
-  </si>
-  <si>
-    <t>-3.38 ± 0.02</t>
-  </si>
-  <si>
-    <t>-377.04 ± 0.83</t>
-  </si>
-  <si>
-    <t>-20.02 ± 0.05</t>
-  </si>
-  <si>
-    <t>-102.43 ± 0.06</t>
-  </si>
-  <si>
-    <t>-4.33 ± 0.01</t>
+    <t>+0.08 ± 0.00</t>
+  </si>
+  <si>
+    <t>-0.09 ± 0.00</t>
+  </si>
+  <si>
+    <t>+509.28 ± 0.75</t>
+  </si>
+  <si>
+    <t>+4.37 ± 0.01</t>
+  </si>
+  <si>
+    <t>-509.37 ± 0.75</t>
+  </si>
+  <si>
+    <t>-3.49 ± 0.02</t>
+  </si>
+  <si>
+    <t>-379.23 ± 0.68</t>
+  </si>
+  <si>
+    <t>-20.08 ± 0.06</t>
+  </si>
+  <si>
+    <t>-102.21 ± 0.06</t>
+  </si>
+  <si>
+    <t>-4.34 ± 0.01</t>
   </si>
   <si>
     <t>+0.94 ± 0.00</t>
   </si>
   <si>
-    <t>+0.68 ± 0.00</t>
-  </si>
-  <si>
-    <t>+26.06 ± 0.04</t>
-  </si>
-  <si>
-    <t>+3.93 ± 0.02</t>
-  </si>
-  <si>
-    <t>+20.16 ± 0.03</t>
-  </si>
-  <si>
-    <t>+1.96 ± 0.01</t>
-  </si>
-  <si>
-    <t>-26.13 ± 0.05</t>
-  </si>
-  <si>
-    <t>-13.94 ± 0.03</t>
-  </si>
-  <si>
-    <t>-0.55 ± 0.00</t>
-  </si>
-  <si>
-    <t>-10.96 ± 0.02</t>
-  </si>
-  <si>
-    <t>-0.68 ± 0.00</t>
-  </si>
-  <si>
-    <t>+0.31 ± 0.00</t>
-  </si>
-  <si>
-    <t>+4.37 ± 0.02</t>
-  </si>
-  <si>
-    <t>+6.42 ± 0.03</t>
-  </si>
-  <si>
-    <t>+3.29 ± 0.02</t>
-  </si>
-  <si>
-    <t>+1.71 ± 0.00</t>
-  </si>
-  <si>
-    <t>+1.41 ± 0.01</t>
-  </si>
-  <si>
-    <t>-6.43 ± 0.03</t>
-  </si>
-  <si>
-    <t>-3.14 ± 0.02</t>
-  </si>
-  <si>
-    <t>-2.99 ± 0.01</t>
+    <t>+0.67 ± 0.00</t>
+  </si>
+  <si>
+    <t>+26.45 ± 0.04</t>
+  </si>
+  <si>
+    <t>+3.84 ± 0.02</t>
+  </si>
+  <si>
+    <t>+20.59 ± 0.02</t>
+  </si>
+  <si>
+    <t>+2.02 ± 0.01</t>
+  </si>
+  <si>
+    <t>-26.52 ± 0.04</t>
+  </si>
+  <si>
+    <t>-14.19 ± 0.02</t>
+  </si>
+  <si>
+    <t>-0.56 ± 0.00</t>
+  </si>
+  <si>
+    <t>-11.08 ± 0.02</t>
+  </si>
+  <si>
+    <t>-0.70 ± 0.00</t>
+  </si>
+  <si>
+    <t>+0.32 ± 0.00</t>
+  </si>
+  <si>
+    <t>+4.39 ± 0.02</t>
+  </si>
+  <si>
+    <t>+6.46 ± 0.03</t>
+  </si>
+  <si>
+    <t>+3.25 ± 0.02</t>
+  </si>
+  <si>
+    <t>+1.75 ± 0.00</t>
+  </si>
+  <si>
+    <t>+1.47 ± 0.01</t>
+  </si>
+  <si>
+    <t>-6.48 ± 0.03</t>
+  </si>
+  <si>
+    <t>-3.17 ± 0.01</t>
+  </si>
+  <si>
+    <t>-0.11 ± 0.00</t>
+  </si>
+  <si>
+    <t>-3.00 ± 0.01</t>
   </si>
   <si>
     <t>-0.20 ± 0.00</t>
@@ -229,7 +232,7 @@
     <t>+0.07 ± 0.00</t>
   </si>
   <si>
-    <t>+3.96 ± 0.04</t>
+    <t>+3.99 ± 0.04</t>
   </si>
 </sst>
 </file>
@@ -814,7 +817,7 @@
         <v>57</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -837,7 +840,7 @@
         <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -860,7 +863,7 @@
         <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -883,7 +886,7 @@
         <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -906,7 +909,7 @@
         <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>